<commit_message>
gpt3.5 with 16K context for k=1,k=3
</commit_message>
<xml_diff>
--- a/graph_generation/results/gpt3.5/level_1/k_3.xlsx
+++ b/graph_generation/results/gpt3.5/level_1/k_3.xlsx
@@ -7,16 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="o_10" sheetId="1" r:id="rId1"/>
-    <sheet name="o_20" sheetId="2" r:id="rId2"/>
-    <sheet name="o_20_jumbled" sheetId="3" r:id="rId3"/>
+    <sheet name="o_20" sheetId="1" r:id="rId1"/>
+    <sheet name="o_20_jumbled" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
   <si>
     <t>prompt</t>
   </si>
@@ -30,80 +29,1143 @@
     <t>evaluator_response</t>
   </si>
   <si>
-    <t xml:space="preserve"> Given is the adjacency matrix for a unweighted undirected graph containing 10 nodes labelled A to J. The value corresponding to each row M and column N represents whether there is a connection between the two nodes, where 0 means no connection.   
+    <t xml:space="preserve"> Given is the adjacency matrix for a unweighted undirected graph containing 20 nodes labelled A to T. The value corresponding to each row M and column N represents whether there is a connection between the two nodes, where 0 means no connection.   
 Consider some examples
-Example 1: What is the shortest path from node A to node K? Return the sequence of nodes in response.
-   A B C D E F G H I J K
- A 0 1 0 0 0 0 0 0 0 0 0
- B 1 0 1 0 0 0 0 0 0 0 0
- C 0 1 0 1 0 0 0 0 0 0 0
- D 0 0 1 0 1 0 0 0 0 0 0
- E 0 0 0 1 0 1 0 0 0 0 0
- F 0 0 0 0 1 0 1 0 0 0 0
- G 0 0 0 0 0 1 0 1 0 0 0
- H 0 0 0 0 0 0 1 0 1 0 0
- I 0 0 0 0 0 0 0 1 0 1 0
- J 0 0 0 0 0 0 0 0 1 0 1
- K 0 0 0 0 0 0 0 0 0 1 0
-Solution: A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J -&gt; K
-Example 2: What is the shortest path from node A to node F? Return the sequence of nodes in response.
-   A B C D E F
- A 0 1 0 0 0 0
- B 1 0 1 0 0 0
- C 0 1 0 1 0 0
- D 0 0 1 0 1 0
- E 0 0 0 1 0 1
- F 0 0 0 0 1 0
-Solution: A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F
-Example 3: What is the shortest path from node A to node I? Return the sequence of nodes in response.
-   A B C D E F G H I
- A 0 1 0 0 0 0 0 0 0
- B 1 0 1 0 0 0 0 0 0
- C 0 1 0 1 0 0 0 0 0
- D 0 0 1 0 1 0 0 0 0
- E 0 0 0 1 0 1 0 0 0
- F 0 0 0 0 1 0 1 0 0
- G 0 0 0 0 0 1 0 1 0
- H 0 0 0 0 0 0 1 0 1
- I 0 0 0 0 0 0 0 1 0
-Solution: A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I
+Example 1: What is the shortest path from node A to node X? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T U V W X
+ A 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ B 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ C 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ E 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ F 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ G 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ H 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ J 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ L 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0
+ N 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0
+ P 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0
+ Q 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0
+ R 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0
+ S 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0
+ T 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0
+ U 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0
+ V 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0
+ W 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1
+ X 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+Solution: A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J -&gt; K -&gt; L -&gt; M -&gt; N -&gt; O -&gt; P -&gt; Q -&gt; R -&gt; S -&gt; T -&gt; U -&gt; V -&gt; W -&gt; X
+Example 2: What is the shortest path from node A to node S? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S
+ A 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ B 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ C 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ E 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ F 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ G 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0
+ H 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0
+ J 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0
+ L 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0
+ N 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0
+ P 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0
+ Q 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0
+ R 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1
+ S 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+Solution: A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J -&gt; K -&gt; L -&gt; M -&gt; N -&gt; O -&gt; P -&gt; Q -&gt; R -&gt; S
+Example 3: What is the shortest path from node A to node Q? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q
+ A 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ B 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ C 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ E 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0
+ F 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0
+ G 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0
+ H 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0
+ J 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0
+ K 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0
+ L 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0
+ N 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0
+ P 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1
+ Q 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+Solution: A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J -&gt; K -&gt; L -&gt; M -&gt; N -&gt; O -&gt; P -&gt; Q
  Given these examples, answer the following quesiton.
-What is the shortest path from node A to node J? Return the sequence of nodes in response.
-   A B C D E F G H I J
- A 0 1 0 0 0 0 0 0 0 0
- B 1 0 1 0 0 0 0 0 0 0
- C 0 1 0 1 0 0 0 0 0 0
- D 0 0 1 0 1 0 0 0 0 0
- E 0 0 0 1 0 1 0 0 0 0
- F 0 0 0 0 1 0 1 0 0 0
- G 0 0 0 0 0 1 0 1 0 0
- H 0 0 0 0 0 0 1 0 1 0
- I 0 0 0 0 0 0 0 1 0 1
- J 0 0 0 0 0 0 0 0 1 0
+What is the shortest path from node A to node T? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T
+ A 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ B 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ C 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ E 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ F 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ G 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ H 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0
+ J 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0
+ L 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0
+ N 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0
+ P 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0
+ Q 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0
+ R 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0
+ S 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1
+ T 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
     </t>
   </si>
   <si>
-    <t>A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J</t>
-  </si>
-  <si>
-    <t>The shortest path from node A to node J is: A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J</t>
-  </si>
-  <si>
-    <t>The shortest path from node A to node J is: A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J.</t>
-  </si>
-  <si>
-    <t>Solution: A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J</t>
-  </si>
-  <si>
-    <t>To find the shortest path from node A to node J, we can use the Breadth-First Search algorithm. Starting from node A, we explore all its neighboring nodes (B) and mark them as visited. Then, we explore the unvisited neighboring nodes of B (C), mark them as visited, and continue this process until we reach node J.
-A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J</t>
-  </si>
-  <si>
-    <t>The shortest path from node A to node J is:
-A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J</t>
+    <t>A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J -&gt; K -&gt; L -&gt; M -&gt; N -&gt; O -&gt; P -&gt; Q -&gt; R -&gt; S -&gt; T</t>
+  </si>
+  <si>
+    <t>The shortest path from node A to node T is: 
+A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J -&gt; K -&gt; L -&gt; M -&gt; N -&gt; O -&gt; P -&gt; Q -&gt; R -&gt; S -&gt; T</t>
+  </si>
+  <si>
+    <t>Solution: A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J -&gt; K -&gt; L -&gt; M -&gt; N -&gt; O -&gt; P -&gt; Q -&gt; R -&gt; S -&gt; T</t>
+  </si>
+  <si>
+    <t>The shortest path from node A to node T is A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J -&gt; K -&gt; L -&gt; M -&gt; N -&gt; O -&gt; P -&gt; Q -&gt; R -&gt; S -&gt; T.</t>
+  </si>
+  <si>
+    <t>The shortest path from node A to node T is: A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J -&gt; K -&gt; L -&gt; M -&gt; N -&gt; O -&gt; P -&gt; Q -&gt; R -&gt; S -&gt; T</t>
+  </si>
+  <si>
+    <t>The shortest path from node A to node T is:
+A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J -&gt; K -&gt; L -&gt; M -&gt; N -&gt; O -&gt; P -&gt; Q -&gt; R -&gt; S -&gt; T</t>
+  </si>
+  <si>
+    <t>The shortest path from node A to node T is:
+A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J -&gt; K -&gt; L -&gt; M -&gt; N -&gt; O -&gt; P -&gt; Q -&gt; R -&gt; S -&gt; T</t>
   </si>
   <si>
     <t>Correct</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Given is the adjacency matrix for a unweighted undirected graph containing 20 nodes labelled A to T. The value corresponding to each row M and column N represents whether there is a connection between the two nodes, where 0 means no connection.   
+Consider some examples
+Example 1: What is the shortest path from node M to node D? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R
+ A 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ B 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0
+ C 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0
+ G 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ H 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0
+ J 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ K 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ L 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ N 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 1 0 0 0 0
+ P 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ Q 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1
+ R 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0
+Solution: M -&gt; K -&gt; P -&gt; B -&gt; H -&gt; A -&gt; C -&gt; G -&gt; N -&gt; O -&gt; I -&gt; L -&gt; F -&gt; E -&gt; Q -&gt; R -&gt; J -&gt; D
+Example 2: What is the shortest path from node K to node O? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S
+ A 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ B 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0
+ C 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0
+ D 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ F 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1
+ G 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ H 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0
+ J 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ L 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ M 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ P 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ R 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0
+ S 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: K -&gt; P -&gt; G -&gt; B -&gt; N -&gt; H -&gt; Q -&gt; A -&gt; M -&gt; C -&gt; D -&gt; J -&gt; F -&gt; S -&gt; E -&gt; L -&gt; R -&gt; I -&gt; O
+Example 3: What is the shortest path from node O to node L? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T U
+ A 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1
+ B 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ C 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 1 0 0 0 0 0
+ D 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ E 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0
+ G 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ H 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+ J 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ L 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ P 0 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ R 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ S 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0
+ T 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ U 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: O -&gt; M -&gt; S -&gt; K -&gt; F -&gt; T -&gt; E -&gt; D -&gt; R -&gt; Q -&gt; A -&gt; U -&gt; B -&gt; N -&gt; H -&gt; J -&gt; C -&gt; P -&gt; I -&gt; G -&gt; L
+ Given these examples, answer the following quesiton.
+What is the shortest path from node O to node T? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T
+ A 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1
+ B 0 0 0 0 0 0 0 1 0 0 0 0 0 1 0 0 0 0 0 0
+ C 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ D 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 1 0 0 0 0
+ F 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ G 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0
+ H 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 1 1 0 0 0 0 0 0 0
+ J 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 1 0
+ K 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ L 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0 0
+ M 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ N 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ O 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ P 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0
+ Q 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0
+ R 0 0 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0
+ S 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0
+ T 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Given is the adjacency matrix for a unweighted undirected graph containing 20 nodes labelled A to T. The value corresponding to each row M and column N represents whether there is a connection between the two nodes, where 0 means no connection.   
+Consider some examples
+Example 1: What is the shortest path from node M to node D? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R
+ A 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ B 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0
+ C 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0
+ G 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ H 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0
+ J 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ K 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ L 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ N 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 1 0 0 0 0
+ P 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ Q 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1
+ R 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0
+Solution: M -&gt; K -&gt; P -&gt; B -&gt; H -&gt; A -&gt; C -&gt; G -&gt; N -&gt; O -&gt; I -&gt; L -&gt; F -&gt; E -&gt; Q -&gt; R -&gt; J -&gt; D
+Example 2: What is the shortest path from node K to node O? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S
+ A 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ B 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0
+ C 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0
+ D 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ F 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1
+ G 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ H 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0
+ J 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ L 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ M 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ P 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ R 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0
+ S 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: K -&gt; P -&gt; G -&gt; B -&gt; N -&gt; H -&gt; Q -&gt; A -&gt; M -&gt; C -&gt; D -&gt; J -&gt; F -&gt; S -&gt; E -&gt; L -&gt; R -&gt; I -&gt; O
+Example 3: What is the shortest path from node O to node L? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T U
+ A 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1
+ B 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ C 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 1 0 0 0 0 0
+ D 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ E 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0
+ G 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ H 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+ J 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ L 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ P 0 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ R 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ S 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0
+ T 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ U 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: O -&gt; M -&gt; S -&gt; K -&gt; F -&gt; T -&gt; E -&gt; D -&gt; R -&gt; Q -&gt; A -&gt; U -&gt; B -&gt; N -&gt; H -&gt; J -&gt; C -&gt; P -&gt; I -&gt; G -&gt; L
+ Given these examples, answer the following quesiton.
+What is the shortest path from node Q to node P? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T
+ A 0 0 0 0 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0
+ B 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0
+ C 0 0 0 0 0 0 0 0 1 0 0 0 0 1 0 0 0 0 0 0
+ D 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0
+ F 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ G 1 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ H 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 1 0
+ I 0 0 1 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ J 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ L 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ M 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ N 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ O 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ P 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ Q 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ R 0 0 0 0 0 0 0 1 0 0 0 0 0 1 0 0 0 0 0 0
+ S 0 0 0 0 0 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0
+ T 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Given is the adjacency matrix for a unweighted undirected graph containing 20 nodes labelled A to T. The value corresponding to each row M and column N represents whether there is a connection between the two nodes, where 0 means no connection.   
+Consider some examples
+Example 1: What is the shortest path from node M to node D? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R
+ A 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ B 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0
+ C 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0
+ G 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ H 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0
+ J 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ K 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ L 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ N 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 1 0 0 0 0
+ P 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ Q 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1
+ R 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0
+Solution: M -&gt; K -&gt; P -&gt; B -&gt; H -&gt; A -&gt; C -&gt; G -&gt; N -&gt; O -&gt; I -&gt; L -&gt; F -&gt; E -&gt; Q -&gt; R -&gt; J -&gt; D
+Example 2: What is the shortest path from node K to node O? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S
+ A 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ B 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0
+ C 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0
+ D 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ F 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1
+ G 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ H 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0
+ J 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ L 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ M 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ P 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ R 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0
+ S 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: K -&gt; P -&gt; G -&gt; B -&gt; N -&gt; H -&gt; Q -&gt; A -&gt; M -&gt; C -&gt; D -&gt; J -&gt; F -&gt; S -&gt; E -&gt; L -&gt; R -&gt; I -&gt; O
+Example 3: What is the shortest path from node O to node L? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T U
+ A 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1
+ B 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ C 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 1 0 0 0 0 0
+ D 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ E 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0
+ G 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ H 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+ J 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ L 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ P 0 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ R 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ S 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0
+ T 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ U 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: O -&gt; M -&gt; S -&gt; K -&gt; F -&gt; T -&gt; E -&gt; D -&gt; R -&gt; Q -&gt; A -&gt; U -&gt; B -&gt; N -&gt; H -&gt; J -&gt; C -&gt; P -&gt; I -&gt; G -&gt; L
+ Given these examples, answer the following quesiton.
+What is the shortest path from node O to node N? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T
+ A 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0
+ B 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0
+ C 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 1 0 0
+ D 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0
+ E 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0
+ F 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0 0
+ G 0 0 0 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ H 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ I 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ J 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 1 0
+ L 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ M 0 0 0 1 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0
+ N 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ P 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ Q 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ R 0 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ S 1 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ T 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Given is the adjacency matrix for a unweighted undirected graph containing 20 nodes labelled A to T. The value corresponding to each row M and column N represents whether there is a connection between the two nodes, where 0 means no connection.   
+Consider some examples
+Example 1: What is the shortest path from node M to node D? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R
+ A 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ B 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0
+ C 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0
+ G 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ H 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0
+ J 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ K 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ L 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ N 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 1 0 0 0 0
+ P 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ Q 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1
+ R 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0
+Solution: M -&gt; K -&gt; P -&gt; B -&gt; H -&gt; A -&gt; C -&gt; G -&gt; N -&gt; O -&gt; I -&gt; L -&gt; F -&gt; E -&gt; Q -&gt; R -&gt; J -&gt; D
+Example 2: What is the shortest path from node K to node O? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S
+ A 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ B 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0
+ C 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0
+ D 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ F 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1
+ G 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ H 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0
+ J 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ L 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ M 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ P 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ R 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0
+ S 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: K -&gt; P -&gt; G -&gt; B -&gt; N -&gt; H -&gt; Q -&gt; A -&gt; M -&gt; C -&gt; D -&gt; J -&gt; F -&gt; S -&gt; E -&gt; L -&gt; R -&gt; I -&gt; O
+Example 3: What is the shortest path from node O to node L? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T U
+ A 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1
+ B 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ C 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 1 0 0 0 0 0
+ D 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ E 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0
+ G 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ H 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+ J 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ L 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ P 0 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ R 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ S 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0
+ T 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ U 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: O -&gt; M -&gt; S -&gt; K -&gt; F -&gt; T -&gt; E -&gt; D -&gt; R -&gt; Q -&gt; A -&gt; U -&gt; B -&gt; N -&gt; H -&gt; J -&gt; C -&gt; P -&gt; I -&gt; G -&gt; L
+ Given these examples, answer the following quesiton.
+What is the shortest path from node E to node I? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T
+ A 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ B 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ C 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0
+ D 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 1
+ E 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ F 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ G 0 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ H 1 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ J 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0
+ K 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ L 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ M 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0 0
+ N 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ O 0 0 0 0 0 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0
+ P 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ Q 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0
+ R 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0
+ S 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0
+ T 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Given is the adjacency matrix for a unweighted undirected graph containing 20 nodes labelled A to T. The value corresponding to each row M and column N represents whether there is a connection between the two nodes, where 0 means no connection.   
+Consider some examples
+Example 1: What is the shortest path from node M to node D? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R
+ A 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ B 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0
+ C 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0
+ G 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ H 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0
+ J 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ K 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ L 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ N 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 1 0 0 0 0
+ P 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ Q 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1
+ R 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0
+Solution: M -&gt; K -&gt; P -&gt; B -&gt; H -&gt; A -&gt; C -&gt; G -&gt; N -&gt; O -&gt; I -&gt; L -&gt; F -&gt; E -&gt; Q -&gt; R -&gt; J -&gt; D
+Example 2: What is the shortest path from node K to node O? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S
+ A 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ B 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0
+ C 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0
+ D 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ F 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1
+ G 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ H 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0
+ J 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ L 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ M 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ P 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ R 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0
+ S 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: K -&gt; P -&gt; G -&gt; B -&gt; N -&gt; H -&gt; Q -&gt; A -&gt; M -&gt; C -&gt; D -&gt; J -&gt; F -&gt; S -&gt; E -&gt; L -&gt; R -&gt; I -&gt; O
+Example 3: What is the shortest path from node O to node L? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T U
+ A 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1
+ B 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ C 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 1 0 0 0 0 0
+ D 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ E 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0
+ G 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ H 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+ J 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ L 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ P 0 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ R 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ S 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0
+ T 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ U 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: O -&gt; M -&gt; S -&gt; K -&gt; F -&gt; T -&gt; E -&gt; D -&gt; R -&gt; Q -&gt; A -&gt; U -&gt; B -&gt; N -&gt; H -&gt; J -&gt; C -&gt; P -&gt; I -&gt; G -&gt; L
+ Given these examples, answer the following quesiton.
+What is the shortest path from node P to node C? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T
+ A 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0
+ B 0 0 0 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0
+ C 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ D 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1
+ E 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 1 0 0 0
+ F 0 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0 0
+ G 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ H 0 1 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ I 0 1 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0
+ J 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 1 0
+ K 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ L 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+ M 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0 0
+ N 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1
+ P 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0
+ Q 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ R 0 0 1 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ S 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ T 0 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Given is the adjacency matrix for a unweighted undirected graph containing 20 nodes labelled A to T. The value corresponding to each row M and column N represents whether there is a connection between the two nodes, where 0 means no connection.   
+Consider some examples
+Example 1: What is the shortest path from node M to node D? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R
+ A 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ B 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0
+ C 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0
+ G 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ H 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0
+ J 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ K 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ L 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ N 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 1 0 0 0 0
+ P 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ Q 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1
+ R 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0
+Solution: M -&gt; K -&gt; P -&gt; B -&gt; H -&gt; A -&gt; C -&gt; G -&gt; N -&gt; O -&gt; I -&gt; L -&gt; F -&gt; E -&gt; Q -&gt; R -&gt; J -&gt; D
+Example 2: What is the shortest path from node K to node O? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S
+ A 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ B 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0
+ C 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0
+ D 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ F 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1
+ G 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ H 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0
+ J 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ L 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ M 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ P 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ R 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0
+ S 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: K -&gt; P -&gt; G -&gt; B -&gt; N -&gt; H -&gt; Q -&gt; A -&gt; M -&gt; C -&gt; D -&gt; J -&gt; F -&gt; S -&gt; E -&gt; L -&gt; R -&gt; I -&gt; O
+Example 3: What is the shortest path from node O to node L? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T U
+ A 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1
+ B 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ C 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 1 0 0 0 0 0
+ D 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ E 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0
+ G 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ H 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+ J 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ L 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ P 0 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ R 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ S 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0
+ T 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ U 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: O -&gt; M -&gt; S -&gt; K -&gt; F -&gt; T -&gt; E -&gt; D -&gt; R -&gt; Q -&gt; A -&gt; U -&gt; B -&gt; N -&gt; H -&gt; J -&gt; C -&gt; P -&gt; I -&gt; G -&gt; L
+ Given these examples, answer the following quesiton.
+What is the shortest path from node J to node F? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T
+ A 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0
+ B 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ C 0 1 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ D 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ F 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ G 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ H 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0
+ I 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ J 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 1 0 0 0
+ L 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0
+ M 0 0 0 0 1 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+ N 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 1 1 0 0 0 0 0 0
+ P 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 1
+ Q 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0
+ R 0 0 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0
+ S 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0
+ T 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Given is the adjacency matrix for a unweighted undirected graph containing 20 nodes labelled A to T. The value corresponding to each row M and column N represents whether there is a connection between the two nodes, where 0 means no connection.   
+Consider some examples
+Example 1: What is the shortest path from node M to node D? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R
+ A 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ B 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0
+ C 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0
+ G 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ H 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0
+ J 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ K 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ L 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ N 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 1 0 0 0 0
+ P 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ Q 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1
+ R 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0
+Solution: M -&gt; K -&gt; P -&gt; B -&gt; H -&gt; A -&gt; C -&gt; G -&gt; N -&gt; O -&gt; I -&gt; L -&gt; F -&gt; E -&gt; Q -&gt; R -&gt; J -&gt; D
+Example 2: What is the shortest path from node K to node O? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S
+ A 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ B 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0
+ C 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0
+ D 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ F 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1
+ G 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ H 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0
+ J 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ L 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ M 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ P 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ R 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0
+ S 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: K -&gt; P -&gt; G -&gt; B -&gt; N -&gt; H -&gt; Q -&gt; A -&gt; M -&gt; C -&gt; D -&gt; J -&gt; F -&gt; S -&gt; E -&gt; L -&gt; R -&gt; I -&gt; O
+Example 3: What is the shortest path from node O to node L? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T U
+ A 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1
+ B 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ C 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 1 0 0 0 0 0
+ D 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ E 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0
+ G 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ H 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+ J 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ L 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ P 0 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ R 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ S 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0
+ T 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ U 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: O -&gt; M -&gt; S -&gt; K -&gt; F -&gt; T -&gt; E -&gt; D -&gt; R -&gt; Q -&gt; A -&gt; U -&gt; B -&gt; N -&gt; H -&gt; J -&gt; C -&gt; P -&gt; I -&gt; G -&gt; L
+ Given these examples, answer the following quesiton.
+What is the shortest path from node L to node S? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T
+ A 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ B 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 1 0 0 0 0
+ C 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ D 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 1 0 0
+ E 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0
+ F 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 1 0
+ G 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ H 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 1 0 0 0 0
+ J 0 0 0 0 0 0 0 0 1 0 0 0 0 1 0 0 0 0 0 0
+ K 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ L 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ N 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0
+ O 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ P 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ Q 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ R 1 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ S 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ T 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0 0 0 0
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Given is the adjacency matrix for a unweighted undirected graph containing 20 nodes labelled A to T. The value corresponding to each row M and column N represents whether there is a connection between the two nodes, where 0 means no connection.   
+Consider some examples
+Example 1: What is the shortest path from node M to node D? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R
+ A 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ B 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0
+ C 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0
+ G 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ H 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0
+ J 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ K 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ L 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ N 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 1 0 0 0 0
+ P 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ Q 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1
+ R 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0
+Solution: M -&gt; K -&gt; P -&gt; B -&gt; H -&gt; A -&gt; C -&gt; G -&gt; N -&gt; O -&gt; I -&gt; L -&gt; F -&gt; E -&gt; Q -&gt; R -&gt; J -&gt; D
+Example 2: What is the shortest path from node K to node O? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S
+ A 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ B 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0
+ C 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0
+ D 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ F 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1
+ G 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ H 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0
+ J 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ L 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ M 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ P 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ R 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0
+ S 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: K -&gt; P -&gt; G -&gt; B -&gt; N -&gt; H -&gt; Q -&gt; A -&gt; M -&gt; C -&gt; D -&gt; J -&gt; F -&gt; S -&gt; E -&gt; L -&gt; R -&gt; I -&gt; O
+Example 3: What is the shortest path from node O to node L? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T U
+ A 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1
+ B 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ C 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 1 0 0 0 0 0
+ D 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ E 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0
+ G 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ H 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+ J 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ L 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ P 0 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ R 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ S 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0
+ T 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ U 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: O -&gt; M -&gt; S -&gt; K -&gt; F -&gt; T -&gt; E -&gt; D -&gt; R -&gt; Q -&gt; A -&gt; U -&gt; B -&gt; N -&gt; H -&gt; J -&gt; C -&gt; P -&gt; I -&gt; G -&gt; L
+ Given these examples, answer the following quesiton.
+What is the shortest path from node B to node F? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T
+ A 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1
+ B 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ C 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0
+ F 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ G 0 0 1 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+ H 0 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+ I 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ J 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ K 0 0 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ L 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0 0
+ M 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ N 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1
+ O 0 0 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0
+ P 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ Q 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ R 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0
+ S 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ T 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Given is the adjacency matrix for a unweighted undirected graph containing 20 nodes labelled A to T. The value corresponding to each row M and column N represents whether there is a connection between the two nodes, where 0 means no connection.   
+Consider some examples
+Example 1: What is the shortest path from node M to node D? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R
+ A 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ B 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0
+ C 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0
+ G 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ H 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0
+ J 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ K 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ L 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ N 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 1 0 0 0 0
+ P 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ Q 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1
+ R 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0
+Solution: M -&gt; K -&gt; P -&gt; B -&gt; H -&gt; A -&gt; C -&gt; G -&gt; N -&gt; O -&gt; I -&gt; L -&gt; F -&gt; E -&gt; Q -&gt; R -&gt; J -&gt; D
+Example 2: What is the shortest path from node K to node O? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S
+ A 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ B 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0
+ C 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0
+ D 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ F 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1
+ G 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ H 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0
+ J 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ L 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ M 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ P 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ R 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0
+ S 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: K -&gt; P -&gt; G -&gt; B -&gt; N -&gt; H -&gt; Q -&gt; A -&gt; M -&gt; C -&gt; D -&gt; J -&gt; F -&gt; S -&gt; E -&gt; L -&gt; R -&gt; I -&gt; O
+Example 3: What is the shortest path from node O to node L? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T U
+ A 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1
+ B 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ C 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 1 0 0 0 0 0
+ D 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ E 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0
+ G 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ H 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+ J 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ L 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ P 0 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ R 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ S 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0
+ T 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ U 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: O -&gt; M -&gt; S -&gt; K -&gt; F -&gt; T -&gt; E -&gt; D -&gt; R -&gt; Q -&gt; A -&gt; U -&gt; B -&gt; N -&gt; H -&gt; J -&gt; C -&gt; P -&gt; I -&gt; G -&gt; L
+ Given these examples, answer the following quesiton.
+What is the shortest path from node L to node E? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T
+ A 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ B 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1
+ C 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0
+ D 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0
+ E 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ F 1 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ G 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0
+ H 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ I 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ J 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0
+ K 0 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ L 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ M 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0
+ N 0 0 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ O 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ P 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0
+ Q 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ R 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ S 0 0 0 0 0 0 0 0 0 0 0 1 1 0 0 0 0 0 0 0
+ T 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Given is the adjacency matrix for a unweighted undirected graph containing 20 nodes labelled A to T. The value corresponding to each row M and column N represents whether there is a connection between the two nodes, where 0 means no connection.   
+Consider some examples
+Example 1: What is the shortest path from node M to node D? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R
+ A 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ B 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0
+ C 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0
+ G 0 0 1 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ H 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0
+ J 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ K 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ L 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ N 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 1 0 0 0 0
+ P 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ Q 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1
+ R 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0
+Solution: M -&gt; K -&gt; P -&gt; B -&gt; H -&gt; A -&gt; C -&gt; G -&gt; N -&gt; O -&gt; I -&gt; L -&gt; F -&gt; E -&gt; Q -&gt; R -&gt; J -&gt; D
+Example 2: What is the shortest path from node K to node O? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S
+ A 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ B 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0
+ C 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0
+ D 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ E 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ F 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1
+ G 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ H 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0 0
+ I 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 1 0
+ J 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ L 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ M 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ P 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ R 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0
+ S 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: K -&gt; P -&gt; G -&gt; B -&gt; N -&gt; H -&gt; Q -&gt; A -&gt; M -&gt; C -&gt; D -&gt; J -&gt; F -&gt; S -&gt; E -&gt; L -&gt; R -&gt; I -&gt; O
+Example 3: What is the shortest path from node O to node L? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T U
+ A 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1
+ B 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1
+ C 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 1 0 0 0 0 0
+ D 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ E 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ F 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0
+ G 0 0 0 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0
+ H 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+ J 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0
+ L 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ N 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0
+ P 0 0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ Q 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0
+ R 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+ S 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0
+ T 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ U 1 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+Solution: O -&gt; M -&gt; S -&gt; K -&gt; F -&gt; T -&gt; E -&gt; D -&gt; R -&gt; Q -&gt; A -&gt; U -&gt; B -&gt; N -&gt; H -&gt; J -&gt; C -&gt; P -&gt; I -&gt; G -&gt; L
+ Given these examples, answer the following quesiton.
+What is the shortest path from node A to node F? Return the sequence of nodes in response.
+   A B C D E F G H I J K L M N O P Q R S T
+ A 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1
+ B 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 1 0
+ C 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 0 0 0 0 0 0 1 0 0 0 0 1 0 0 0 0 0 0
+ E 0 0 1 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0
+ F 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ G 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+ H 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0
+ I 0 0 0 1 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0
+ J 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0 0
+ K 0 0 0 0 0 1 0 0 1 0 0 0 0 0 0 0 0 0 0 0
+ L 0 1 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0
+ M 0 0 0 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0
+ N 0 0 0 1 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 1 0 0 0 0
+ P 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 1
+ Q 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 0
+ R 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 1 0 0 0
+ S 0 1 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ T 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0
+    </t>
+  </si>
+  <si>
+    <t>O -&gt; E -&gt; P -&gt; N -&gt; B -&gt; H -&gt; R -&gt; G -&gt; J -&gt; S -&gt; Q -&gt; L -&gt; I -&gt; M -&gt; F -&gt; D -&gt; C -&gt; K -&gt; A -&gt; T</t>
+  </si>
+  <si>
+    <t>Q -&gt; K -&gt; E -&gt; J -&gt; D -&gt; F -&gt; T -&gt; O -&gt; B -&gt; M -&gt; S -&gt; H -&gt; R -&gt; N -&gt; C -&gt; I -&gt; G -&gt; A -&gt; L -&gt; P</t>
+  </si>
+  <si>
+    <t>O -&gt; T -&gt; Q -&gt; B -&gt; H -&gt; C -&gt; R -&gt; I -&gt; E -&gt; P -&gt; L -&gt; A -&gt; S -&gt; K -&gt; G -&gt; F -&gt; J -&gt; D -&gt; M -&gt; N</t>
+  </si>
+  <si>
+    <t>E -&gt; B -&gt; P -&gt; T -&gt; D -&gt; H -&gt; A -&gt; F -&gt; G -&gt; M -&gt; R -&gt; K -&gt; O -&gt; J -&gt; S -&gt; N -&gt; C -&gt; L -&gt; Q -&gt; I</t>
+  </si>
+  <si>
+    <t>P -&gt; N -&gt; I -&gt; B -&gt; H -&gt; F -&gt; L -&gt; O -&gt; T -&gt; D -&gt; Q -&gt; E -&gt; G -&gt; M -&gt; J -&gt; S -&gt; A -&gt; K -&gt; R -&gt; C</t>
+  </si>
+  <si>
+    <t>J -&gt; H -&gt; R -&gt; G -&gt; A -&gt; N -&gt; O -&gt; M -&gt; E -&gt; T -&gt; P -&gt; S -&gt; L -&gt; K -&gt; Q -&gt; I -&gt; D -&gt; B -&gt; C -&gt; F</t>
+  </si>
+  <si>
+    <t>L -&gt; C -&gt; A -&gt; R -&gt; D -&gt; Q -&gt; M -&gt; E -&gt; K -&gt; H -&gt; N -&gt; J -&gt; I -&gt; P -&gt; B -&gt; O -&gt; T -&gt; G -&gt; F -&gt; S</t>
+  </si>
+  <si>
+    <t>B -&gt; J -&gt; K -&gt; D -&gt; H -&gt; O -&gt; G -&gt; C -&gt; I -&gt; L -&gt; Q -&gt; A -&gt; T -&gt; N -&gt; R -&gt; P -&gt; E -&gt; S -&gt; M -&gt; F</t>
+  </si>
+  <si>
+    <t>L -&gt; S -&gt; M -&gt; K -&gt; B -&gt; T -&gt; O -&gt; C -&gt; H -&gt; Q -&gt; D -&gt; N -&gt; J -&gt; A -&gt; F -&gt; I -&gt; P -&gt; G -&gt; R -&gt; E</t>
+  </si>
+  <si>
+    <t>A -&gt; T -&gt; P -&gt; O -&gt; L -&gt; B -&gt; S -&gt; G -&gt; C -&gt; E -&gt; M -&gt; J -&gt; Q -&gt; R -&gt; H -&gt; N -&gt; D -&gt; I -&gt; K -&gt; F</t>
+  </si>
+  <si>
+    <t>The shortest path from node O to node T is: O -&gt; M -&gt; L -&gt; R -&gt; S -&gt; T</t>
+  </si>
+  <si>
+    <t>The shortest path from node Q to node P is Q -&gt; K -&gt; F -&gt; S -&gt; G -&gt; H -&gt; A -&gt; M -&gt; C -&gt; J -&gt; D -&gt; P.</t>
+  </si>
+  <si>
+    <t>The shortest path from node O to node N is: O -&gt; M -&gt; N</t>
+  </si>
+  <si>
+    <t>The shortest path from node E to node I is: E -&gt; B -&gt; Q -&gt; I</t>
+  </si>
+  <si>
+    <t>The shortest path from node P to node C is: 
+P -&gt; B -&gt; H -&gt; J -&gt; C</t>
+  </si>
+  <si>
+    <t>The shortest path from node J to node F is J -&gt; A -&gt; G -&gt; C -&gt; F.</t>
+  </si>
+  <si>
+    <t>Solution: L -&gt; C -&gt; R -&gt; D -&gt; E -&gt; F -&gt; G -&gt; S</t>
+  </si>
+  <si>
+    <t>The shortest path from node B to node F is:
+B -&gt; I -&gt; J -&gt; F</t>
+  </si>
+  <si>
+    <t>The shortest path from node L to node E is L -&gt; S -&gt; F -&gt; E.</t>
+  </si>
+  <si>
+    <t>Solution: A -&gt; B -&gt; L -&gt; F</t>
+  </si>
+  <si>
+    <t>Wrong</t>
   </si>
 </sst>
 </file>
@@ -492,7 +1554,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -506,7 +1568,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -517,10 +1579,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -534,7 +1596,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -545,10 +1607,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -559,10 +1621,10 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -573,10 +1635,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -587,10 +1649,10 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -601,10 +1663,10 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -618,7 +1680,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -628,7 +1690,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -648,31 +1710,144 @@
         <v>3</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>